<commit_message>
Fix failed to be parsed values
</commit_message>
<xml_diff>
--- a/references/Zoning_Parser_Codebook.xlsx
+++ b/references/Zoning_Parser_Codebook.xlsx
@@ -9,15 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="prefix" sheetId="4" r:id="rId1"/>
-    <sheet name="zone_class" sheetId="3" r:id="rId2"/>
-    <sheet name="height_district" sheetId="6" r:id="rId3"/>
-    <sheet name="supplemental_use_overlay" sheetId="1" r:id="rId4"/>
-    <sheet name="specific_plan" sheetId="2" r:id="rId5"/>
-    <sheet name="special_cases" sheetId="5" r:id="rId6"/>
+    <sheet name="zone_class" sheetId="3" r:id="rId1"/>
+    <sheet name="height_district" sheetId="6" r:id="rId2"/>
+    <sheet name="supplemental_use_overlay" sheetId="1" r:id="rId3"/>
+    <sheet name="specific_plan" sheetId="2" r:id="rId4"/>
+    <sheet name="use_for_parse_fails" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="317">
   <si>
     <t>O</t>
   </si>
@@ -268,9 +267,6 @@
     <t>usc_university_park_campus_specific_plan_subarea_2_zone</t>
   </si>
   <si>
-    <t>usc_university_park_campus_specific_plan_subarea_3_zone</t>
-  </si>
-  <si>
     <t>zone_class</t>
   </si>
   <si>
@@ -520,9 +516,6 @@
     <t>(WC)UPTOWN</t>
   </si>
   <si>
-    <t>zone_cmplt</t>
-  </si>
-  <si>
     <t>warner_center_college</t>
   </si>
   <si>
@@ -550,18 +543,12 @@
     <t>urban_village</t>
   </si>
   <si>
-    <t>specific plan? Overlay? It's usage and placement looks like specific plan…not 100% sure</t>
-  </si>
-  <si>
     <t>expo_corridor</t>
   </si>
   <si>
     <t>paramount_pictures_specific_plan</t>
   </si>
   <si>
-    <t>might want to move some of the specific plans into special cases, because they have extra zone_class info that we otherwise wouldn't know</t>
-  </si>
-  <si>
     <t>agricultural</t>
   </si>
   <si>
@@ -782,13 +769,223 @@
   </si>
   <si>
     <t>height_and_d_limit</t>
+  </si>
+  <si>
+    <t>SP</t>
+  </si>
+  <si>
+    <t>NMU</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>neighborhood_mixed_use</t>
+  </si>
+  <si>
+    <t>unknown1</t>
+  </si>
+  <si>
+    <t>unknown2</t>
+  </si>
+  <si>
+    <t>ZONE_CMPLT</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>overlay</t>
+  </si>
+  <si>
+    <t>(WC)TOPANGA-SN-RIO</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>[SN, RIO]</t>
+  </si>
+  <si>
+    <t>[Q]RZ5-1</t>
+  </si>
+  <si>
+    <t>RZ5</t>
+  </si>
+  <si>
+    <t>A2P-1</t>
+  </si>
+  <si>
+    <t>A2P</t>
+  </si>
+  <si>
+    <t>(T)(Q)RZ5-1</t>
+  </si>
+  <si>
+    <t>(F)CM-1-CUGU</t>
+  </si>
+  <si>
+    <t>[CUGU]</t>
+  </si>
+  <si>
+    <t>(F)CM-1-HPOZ</t>
+  </si>
+  <si>
+    <t>[HPOZ]</t>
+  </si>
+  <si>
+    <t>(F)CM-1-O-HPOZ</t>
+  </si>
+  <si>
+    <t>[O, HPOZ]</t>
+  </si>
+  <si>
+    <t>(F)R2-1-RIO</t>
+  </si>
+  <si>
+    <t>[RIO]</t>
+  </si>
+  <si>
+    <t>(F)RE11-1</t>
+  </si>
+  <si>
+    <t>UV(CA)</t>
+  </si>
+  <si>
+    <t>[CA]</t>
+  </si>
+  <si>
+    <t>UC(CA)-CDO</t>
+  </si>
+  <si>
+    <t>UC</t>
+  </si>
+  <si>
+    <t>UC(CA)</t>
+  </si>
+  <si>
+    <t>UI(CA)</t>
+  </si>
+  <si>
+    <t>LACFCD</t>
+  </si>
+  <si>
+    <t>(WC)PARK-SN</t>
+  </si>
+  <si>
+    <t>[SN]</t>
+  </si>
+  <si>
+    <t>R1-1XL-O#-CUGU</t>
+  </si>
+  <si>
+    <t>[O, CUGU]</t>
+  </si>
+  <si>
+    <t>(WC)TOPANGA-SN</t>
+  </si>
+  <si>
+    <t>(WC)COMMERCE-SN</t>
+  </si>
+  <si>
+    <t>(WC)DOWNTOWN-SN</t>
+  </si>
+  <si>
+    <t>(WC)COLLEGE-SN</t>
+  </si>
+  <si>
+    <t>(WC)NORTHVILLAGE-SN-RIO</t>
+  </si>
+  <si>
+    <t>(WC)UPTOWN-SN-RIO</t>
+  </si>
+  <si>
+    <t>VARIOUS</t>
+  </si>
+  <si>
+    <t>RE15-1-H#</t>
+  </si>
+  <si>
+    <t>[H]</t>
+  </si>
+  <si>
+    <t>RE15-1-RPD-2.9-H</t>
+  </si>
+  <si>
+    <t>[RPD]</t>
+  </si>
+  <si>
+    <t>M(PV)</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>(WC)RIVER-SN-RIO</t>
+  </si>
+  <si>
+    <t>MU(EC)</t>
+  </si>
+  <si>
+    <t>[MU]</t>
+  </si>
+  <si>
+    <t>UV, CA</t>
+  </si>
+  <si>
+    <t>UI, CA</t>
+  </si>
+  <si>
+    <t>UC, CA</t>
+  </si>
+  <si>
+    <t>[CDO]</t>
+  </si>
+  <si>
+    <t>cornfield_arroyo_seco_specific_plan</t>
+  </si>
+  <si>
+    <t>[Q]CCS-O</t>
+  </si>
+  <si>
+    <t>ADP-RIO</t>
+  </si>
+  <si>
+    <t>(Q)CEC-4D-O</t>
+  </si>
+  <si>
+    <t>MU(EC)-O</t>
+  </si>
+  <si>
+    <t>NMU(EC)-O-POD</t>
+  </si>
+  <si>
+    <t>NMU(EC)-POD</t>
+  </si>
+  <si>
+    <t>[O]</t>
+  </si>
+  <si>
+    <t>[MU, O]</t>
+  </si>
+  <si>
+    <t>[NMU, POD]</t>
+  </si>
+  <si>
+    <t>[NMU, O, POD]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -798,6 +995,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -818,7 +1023,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -835,19 +1040,33 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1128,973 +1347,959 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="50.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" t="s">
         <v>80</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>81</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="D1" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>83</v>
-      </c>
       <c r="B2" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C2" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="D2">
         <v>201</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>84</v>
+      <c r="A3" s="3" t="s">
+        <v>83</v>
       </c>
       <c r="B3" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C3" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="D3">
         <v>202</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>85</v>
+      <c r="A4" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="B4" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C4" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="D4">
         <v>204</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>86</v>
+      <c r="A5" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="B5" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C5" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D5">
         <v>306</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>87</v>
+      <c r="A6" s="3" t="s">
+        <v>86</v>
       </c>
       <c r="B6" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C6" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D6">
         <v>301</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>88</v>
+      <c r="A7" s="3" t="s">
+        <v>87</v>
       </c>
       <c r="B7" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C7" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D7">
         <v>302</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>89</v>
+      <c r="A8" s="3" t="s">
+        <v>88</v>
       </c>
       <c r="B8" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C8" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D8">
         <v>303</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>90</v>
+      <c r="A9" s="3" t="s">
+        <v>89</v>
       </c>
       <c r="B9" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C9" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D9">
         <v>304</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>91</v>
+      <c r="A10" s="3" t="s">
+        <v>90</v>
       </c>
       <c r="B10" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C10" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D10">
         <v>305</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>92</v>
+      <c r="A11" s="3" t="s">
+        <v>91</v>
       </c>
       <c r="B11" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C11" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D11">
         <v>307</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>93</v>
+      <c r="A12" s="3" t="s">
+        <v>92</v>
       </c>
       <c r="B12" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C12" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D12">
         <v>308</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B13" t="s">
+        <v>193</v>
+      </c>
+      <c r="C13" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B13" t="s">
-        <v>197</v>
-      </c>
-      <c r="C13" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="B14" t="s">
+        <v>193</v>
+      </c>
+      <c r="C14" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B14" t="s">
-        <v>197</v>
-      </c>
-      <c r="C14" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="B15" t="s">
+        <v>193</v>
+      </c>
+      <c r="C15" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B16" t="s">
+        <v>193</v>
+      </c>
+      <c r="C16" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B15" t="s">
-        <v>197</v>
-      </c>
-      <c r="C15" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="B16" t="s">
-        <v>197</v>
-      </c>
-      <c r="C16" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>97</v>
-      </c>
       <c r="B17" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C17" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D17">
         <v>309</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>98</v>
+      <c r="A18" s="3" t="s">
+        <v>97</v>
       </c>
       <c r="B18" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C18" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D18">
         <v>310</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>99</v>
+      <c r="A19" s="3" t="s">
+        <v>98</v>
       </c>
       <c r="B19" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C19" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D19">
         <v>311</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>100</v>
+      <c r="A20" s="3" t="s">
+        <v>99</v>
       </c>
       <c r="B20" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C20" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D20">
         <v>312</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>101</v>
+      <c r="A21" s="3" t="s">
+        <v>100</v>
       </c>
       <c r="B21" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="C21" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D21">
         <v>314</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>102</v>
+      <c r="A22" s="3" t="s">
+        <v>101</v>
       </c>
       <c r="B22" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C22" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="D22">
         <v>401</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>103</v>
+      <c r="A23" s="3" t="s">
+        <v>102</v>
       </c>
       <c r="B23" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C23" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="D23">
         <v>402</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>104</v>
+      <c r="A24" s="3" t="s">
+        <v>103</v>
       </c>
       <c r="B24" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C24" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="D24">
         <v>403</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
-        <v>105</v>
+      <c r="A25" s="3" t="s">
+        <v>104</v>
       </c>
       <c r="B25" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C25" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="D25">
         <v>404</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
-        <v>106</v>
+      <c r="A26" s="3" t="s">
+        <v>105</v>
       </c>
       <c r="B26" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C26" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="D26">
         <v>405</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
-        <v>107</v>
+      <c r="A27" s="3" t="s">
+        <v>106</v>
       </c>
       <c r="B27" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="C27" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="D27">
         <v>406</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
-        <v>108</v>
+      <c r="A28" s="3" t="s">
+        <v>107</v>
       </c>
       <c r="B28" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C28" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="D28">
         <v>407</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
-        <v>109</v>
+      <c r="A29" s="3" t="s">
+        <v>108</v>
       </c>
       <c r="B29" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="C29" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="D29">
         <v>408</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
-        <v>110</v>
+      <c r="A30" s="3" t="s">
+        <v>109</v>
       </c>
       <c r="B30" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C30" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="D30">
         <v>409</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
-        <v>111</v>
+      <c r="A31" s="3" t="s">
+        <v>110</v>
       </c>
       <c r="B31" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C31" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="D31">
         <v>410</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
-        <v>112</v>
+      <c r="A32" s="3" t="s">
+        <v>111</v>
       </c>
       <c r="B32" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="C32" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="D32">
         <v>415</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
-        <v>113</v>
+      <c r="A33" s="3" t="s">
+        <v>112</v>
       </c>
       <c r="B33" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C33" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="D33">
         <v>412</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
-        <v>114</v>
+      <c r="A34" s="3" t="s">
+        <v>113</v>
       </c>
       <c r="B34" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="C34" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="D34">
         <v>416</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
-        <v>115</v>
+      <c r="A35" s="3" t="s">
+        <v>114</v>
       </c>
       <c r="B35" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C35" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="D35">
         <v>414</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
-        <v>116</v>
+      <c r="A36" s="3" t="s">
+        <v>115</v>
       </c>
       <c r="B36" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C36" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D36">
         <v>318</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
-        <v>117</v>
+      <c r="A37" s="3" t="s">
+        <v>116</v>
       </c>
       <c r="B37" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C37" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D37">
         <v>319</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
-        <v>118</v>
+      <c r="A38" s="3" t="s">
+        <v>117</v>
       </c>
       <c r="B38" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C38" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D38">
         <v>315</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
-        <v>119</v>
+      <c r="A39" s="3" t="s">
+        <v>118</v>
       </c>
       <c r="B39" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C39" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D39">
         <v>316</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="4" t="s">
-        <v>120</v>
+      <c r="A40" s="3" t="s">
+        <v>119</v>
       </c>
       <c r="B40" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C40" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D40">
         <v>317</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="4" t="s">
-        <v>121</v>
+      <c r="A41" s="3" t="s">
+        <v>120</v>
       </c>
       <c r="B41" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C41" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="D41">
         <v>601</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="4" t="s">
-        <v>122</v>
+      <c r="A42" s="3" t="s">
+        <v>121</v>
       </c>
       <c r="B42" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C42" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="D42">
         <v>603</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="4" t="s">
-        <v>123</v>
+      <c r="A43" s="3" t="s">
+        <v>122</v>
       </c>
       <c r="B43" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C43" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="D43">
         <v>605</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="4" t="s">
-        <v>124</v>
+      <c r="A44" s="3" t="s">
+        <v>123</v>
       </c>
       <c r="B44" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C44" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="D44">
         <v>606</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="4" t="s">
-        <v>125</v>
+      <c r="A45" s="3" t="s">
+        <v>124</v>
       </c>
       <c r="B45" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C45" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="D45">
         <v>608</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="4" t="s">
-        <v>126</v>
+      <c r="A46" s="3" t="s">
+        <v>125</v>
       </c>
       <c r="B46" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C46" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="D46">
         <v>611</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="4" t="s">
-        <v>127</v>
+      <c r="A47" s="3" t="s">
+        <v>126</v>
       </c>
       <c r="B47" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C47" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="D47">
         <v>701</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="4" t="s">
-        <v>128</v>
+      <c r="A48" s="3" t="s">
+        <v>127</v>
       </c>
       <c r="B48" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="C48" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="D48">
         <v>703</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="4" t="s">
-        <v>129</v>
+      <c r="A49" s="3" t="s">
+        <v>128</v>
       </c>
       <c r="B49" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="C49" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="D49">
         <v>707</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="4" t="s">
-        <v>130</v>
+      <c r="A50" s="3" t="s">
+        <v>129</v>
       </c>
       <c r="B50" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="C50" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="D50">
         <v>705</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="4" t="s">
-        <v>131</v>
+      <c r="A51" s="3" t="s">
+        <v>130</v>
       </c>
       <c r="B51" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="C51" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="D51">
         <v>708</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="4" t="s">
-        <v>132</v>
+      <c r="A52" s="3" t="s">
+        <v>131</v>
       </c>
       <c r="B52" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C52" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="D52">
         <v>710</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="4" t="s">
-        <v>133</v>
+      <c r="A53" s="3" t="s">
+        <v>132</v>
       </c>
       <c r="B53" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C53" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D53">
         <v>501</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="4" t="s">
-        <v>134</v>
+      <c r="A54" s="3" t="s">
+        <v>133</v>
       </c>
       <c r="B54" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C54" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D54">
         <v>518</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="4" t="s">
-        <v>135</v>
+      <c r="A55" s="3" t="s">
+        <v>134</v>
       </c>
       <c r="B55" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C55" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D55">
         <v>507</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="4" t="s">
-        <v>136</v>
+      <c r="A56" s="3" t="s">
+        <v>135</v>
       </c>
       <c r="B56" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C56" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D56">
         <v>508</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="4" t="s">
-        <v>137</v>
+      <c r="A57" s="3" t="s">
+        <v>136</v>
       </c>
       <c r="B57" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C57" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D57">
         <v>515</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="4" t="s">
-        <v>138</v>
+      <c r="A58" s="3" t="s">
+        <v>137</v>
       </c>
       <c r="B58" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C58" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D58">
         <v>516</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="4" t="s">
-        <v>139</v>
+      <c r="A59" s="3" t="s">
+        <v>138</v>
       </c>
       <c r="B59" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C59" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D59">
         <v>517</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="4" t="s">
-        <v>140</v>
+      <c r="A60" s="3" t="s">
+        <v>139</v>
       </c>
       <c r="B60" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C60" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D60">
         <v>505</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="4" t="s">
-        <v>141</v>
+      <c r="A61" s="3" t="s">
+        <v>140</v>
       </c>
       <c r="B61" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C61" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D61">
         <v>506</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="4" t="s">
-        <v>142</v>
+      <c r="A62" s="3" t="s">
+        <v>141</v>
       </c>
       <c r="B62" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="C62" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D62">
         <v>101</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="4" t="s">
+      <c r="A63" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B63" t="s">
+        <v>219</v>
+      </c>
+      <c r="C63" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="B63" t="s">
-        <v>223</v>
-      </c>
-      <c r="C63" t="s">
+      <c r="B64" t="s">
+        <v>220</v>
+      </c>
+      <c r="C64" t="s">
         <v>150</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="B64" t="s">
-        <v>224</v>
-      </c>
-      <c r="C64" t="s">
-        <v>151</v>
       </c>
       <c r="D64">
         <v>801</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="4" t="s">
-        <v>145</v>
+      <c r="A65" s="3" t="s">
+        <v>144</v>
       </c>
       <c r="B65" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="C65" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D65">
         <v>803</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="4" t="s">
-        <v>146</v>
+      <c r="A66" s="3" t="s">
+        <v>145</v>
       </c>
       <c r="B66" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C66" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D66">
         <v>711</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="4" t="s">
+      <c r="A67" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B67" t="s">
+        <v>223</v>
+      </c>
+      <c r="C67" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="B67" t="s">
-        <v>227</v>
-      </c>
-      <c r="C67" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="4" t="s">
+      <c r="B68" t="s">
+        <v>224</v>
+      </c>
+      <c r="C68" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="B68" t="s">
-        <v>228</v>
-      </c>
-      <c r="C68" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="4" t="s">
-        <v>149</v>
-      </c>
       <c r="B69" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="C69" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -2103,13 +2308,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2119,189 +2322,189 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B1" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="C1" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="C2" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="C3" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="B4" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="C4" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B5" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="C5" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B6" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="C6" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B7" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="C7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="B8" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C8" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="B9" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C9" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="B10" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="C10" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>234</v>
+      </c>
+      <c r="B11" t="s">
+        <v>233</v>
+      </c>
+      <c r="C11" t="s">
         <v>238</v>
-      </c>
-      <c r="B11" t="s">
-        <v>237</v>
-      </c>
-      <c r="C11" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="C12" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="C13" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="C14" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="C15" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C16" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C17" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
   </sheetData>
@@ -2310,12 +2513,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2500,17 +2703,41 @@
         <v>41</v>
       </c>
     </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>247</v>
+      </c>
+      <c r="B23" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>248</v>
+      </c>
+      <c r="B24" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>249</v>
+      </c>
+      <c r="B25" t="s">
+        <v>252</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2519,7 +2746,7 @@
     <col min="2" max="2" width="56.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>44</v>
       </c>
@@ -2527,7 +2754,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>46</v>
       </c>
@@ -2535,7 +2762,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>47</v>
       </c>
@@ -2543,7 +2770,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>48</v>
       </c>
@@ -2551,7 +2778,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>49</v>
       </c>
@@ -2559,7 +2786,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>50</v>
       </c>
@@ -2567,7 +2794,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>51</v>
       </c>
@@ -2575,7 +2802,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>52</v>
       </c>
@@ -2583,7 +2810,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>53</v>
       </c>
@@ -2591,7 +2818,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>54</v>
       </c>
@@ -2599,7 +2826,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>55</v>
       </c>
@@ -2607,7 +2834,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>56</v>
       </c>
@@ -2615,7 +2842,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>57</v>
       </c>
@@ -2623,7 +2850,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>62</v>
       </c>
@@ -2631,228 +2858,1279 @@
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>58</v>
+      </c>
+      <c r="B15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>154</v>
+      </c>
+      <c r="B19" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>155</v>
+      </c>
+      <c r="B20" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>156</v>
+      </c>
+      <c r="B21" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>157</v>
+      </c>
+      <c r="B22" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>158</v>
+      </c>
+      <c r="B23" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>159</v>
+      </c>
+      <c r="B24" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>160</v>
+      </c>
+      <c r="B25" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>161</v>
+      </c>
+      <c r="B26" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>151</v>
+      </c>
+      <c r="B27" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B28" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B29" t="s">
         <v>172</v>
       </c>
-      <c r="C15" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="B16" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="B17" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C19" s="7" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="2"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="2"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="2"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="2"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="2"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" t="s">
+        <v>306</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:H61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="56.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.5703125" style="13" customWidth="1"/>
+    <col min="2" max="3" width="9.140625" style="6"/>
+    <col min="4" max="4" width="10.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>163</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E1" t="s">
-        <v>81</v>
-      </c>
-      <c r="F1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="F1" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="B2" s="6">
+        <v>0</v>
+      </c>
+      <c r="C2" s="6">
+        <v>0</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="G2" s="6">
+        <v>0</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="6">
+        <v>0</v>
+      </c>
+      <c r="C3" s="6">
+        <v>0</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="G3" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="B4" s="6">
+        <v>1</v>
+      </c>
+      <c r="C4" s="6">
+        <v>0</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="G4" s="6">
+        <v>0</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="B5" s="6">
+        <v>0</v>
+      </c>
+      <c r="C5" s="6">
+        <v>0</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="G5" s="6">
+        <v>0</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="B6" s="6">
+        <v>1</v>
+      </c>
+      <c r="C6" s="6">
+        <v>1</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="G6" s="6">
+        <v>0</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="B7" s="6">
+        <v>0</v>
+      </c>
+      <c r="C7" s="6">
+        <v>1</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="G7" s="6">
+        <v>0</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="B8" s="6">
+        <v>0</v>
+      </c>
+      <c r="C8" s="6">
+        <v>1</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="G8" s="6">
+        <v>0</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="B9" s="6">
+        <v>0</v>
+      </c>
+      <c r="C9" s="6">
+        <v>1</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="G9" s="6">
+        <v>0</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="B10" s="6">
+        <v>0</v>
+      </c>
+      <c r="C10" s="6">
+        <v>0</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="G10" s="6">
+        <v>0</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="B11" s="6">
+        <v>0</v>
+      </c>
+      <c r="C11" s="6">
+        <v>0</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="G11" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>275</v>
+      </c>
+      <c r="B12" s="10">
+        <v>0</v>
+      </c>
+      <c r="C12" s="10">
+        <v>0</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>302</v>
+      </c>
+      <c r="G12" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="B13" s="10">
+        <v>0</v>
+      </c>
+      <c r="C13" s="10">
+        <v>0</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="G13" s="10">
+        <v>0</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B14" s="6">
+        <v>0</v>
+      </c>
+      <c r="C14" s="6">
+        <v>0</v>
+      </c>
+      <c r="E14" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="G14" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>279</v>
+      </c>
+      <c r="B15" s="10">
+        <v>0</v>
+      </c>
+      <c r="C15" s="10">
+        <v>0</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>278</v>
+      </c>
+      <c r="G15" s="10">
+        <v>0</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" s="6">
+        <v>0</v>
+      </c>
+      <c r="C16" s="6">
+        <v>0</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="G16" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B17" s="6">
+        <v>0</v>
+      </c>
+      <c r="C17" s="6">
+        <v>0</v>
+      </c>
+      <c r="E17" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="G17" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="B18" s="10">
+        <v>0</v>
+      </c>
+      <c r="C18" s="10">
+        <v>0</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>303</v>
+      </c>
+      <c r="G18" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="B19" s="6">
+        <v>0</v>
+      </c>
+      <c r="C19" s="6">
+        <v>0</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="G19" s="6">
+        <v>0</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" s="6">
+        <v>0</v>
+      </c>
+      <c r="C20" s="6">
+        <v>0</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="G20" s="6">
+        <v>0</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" s="6">
+        <v>0</v>
+      </c>
+      <c r="C21" s="6">
+        <v>0</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="G21" s="6">
+        <v>0</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="B22" s="6">
+        <v>0</v>
+      </c>
+      <c r="C22" s="6">
+        <v>0</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="G22" s="6">
+        <v>0</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B23" s="6">
+        <v>0</v>
+      </c>
+      <c r="C23" s="6">
+        <v>0</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="G23" s="6">
+        <v>0</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="B24" s="6">
+        <v>0</v>
+      </c>
+      <c r="C24" s="6">
+        <v>0</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="G24" s="6">
+        <v>0</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25" s="6">
+        <v>0</v>
+      </c>
+      <c r="C25" s="6">
+        <v>0</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="G25" s="6">
+        <v>0</v>
+      </c>
+      <c r="H25" s="6" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="B26" s="6">
+        <v>0</v>
+      </c>
+      <c r="C26" s="6">
+        <v>0</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="G26" s="6">
+        <v>0</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
+        <v>287</v>
+      </c>
+      <c r="B27" s="6">
+        <v>0</v>
+      </c>
+      <c r="C27" s="6">
+        <v>1</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="E27" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C6" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="F27" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="G27" s="6">
+        <v>0</v>
+      </c>
+      <c r="H27" s="6" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="B28" s="6">
+        <v>0</v>
+      </c>
+      <c r="C28" s="6">
+        <v>0</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="E28" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="C7" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="F28" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="G28" s="6">
+        <v>0</v>
+      </c>
+      <c r="H28" s="6" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
+        <v>289</v>
+      </c>
+      <c r="B29" s="6">
+        <v>0</v>
+      </c>
+      <c r="C29" s="6">
+        <v>1</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="G29" s="6">
+        <v>0</v>
+      </c>
+      <c r="H29" s="6" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="B30" s="6">
+        <v>0</v>
+      </c>
+      <c r="C30" s="6">
+        <v>0</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="E30" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="C8" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="C9" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="F30" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="G30" s="6">
+        <v>0</v>
+      </c>
+      <c r="H30" s="6" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="7" t="s">
+        <v>291</v>
+      </c>
+      <c r="B31" s="6">
+        <v>0</v>
+      </c>
+      <c r="C31" s="6">
+        <v>0</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="G31" s="6">
+        <v>0</v>
+      </c>
+      <c r="H31" s="6" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="7" t="s">
+        <v>292</v>
+      </c>
+      <c r="G32" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="B33" s="6">
+        <v>0</v>
+      </c>
+      <c r="C33" s="6">
+        <v>0</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="F33" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="G33" s="6">
+        <v>0</v>
+      </c>
+      <c r="H33" s="6" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="B34" s="12">
+        <v>0</v>
+      </c>
+      <c r="C34" s="12">
+        <v>0</v>
+      </c>
+      <c r="D34" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="F34" s="12" t="s">
+        <v>259</v>
+      </c>
+      <c r="G34" s="12">
+        <v>0</v>
+      </c>
+      <c r="H34" s="12" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="7" t="s">
+        <v>297</v>
+      </c>
+      <c r="B35" s="6">
+        <v>0</v>
+      </c>
+      <c r="C35" s="6">
+        <v>0</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>298</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="G35" s="6">
+        <v>0</v>
+      </c>
+      <c r="H35" s="6" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="B36" s="6">
+        <v>0</v>
+      </c>
+      <c r="C36" s="6">
+        <v>0</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="E36" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="C10" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="C11" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="C12" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="C13" t="s">
-        <v>170</v>
-      </c>
+      <c r="F36" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="G36" s="6">
+        <v>0</v>
+      </c>
+      <c r="H36" s="6" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="9" t="s">
+        <v>300</v>
+      </c>
+      <c r="B37" s="10">
+        <v>0</v>
+      </c>
+      <c r="C37" s="10">
+        <v>0</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>259</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="F37" s="10" t="s">
+        <v>259</v>
+      </c>
+      <c r="G37" s="10">
+        <v>0</v>
+      </c>
+      <c r="H37" s="10" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="B38" s="6">
+        <v>0</v>
+      </c>
+      <c r="C38" s="6">
+        <v>0</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="G38" s="6">
+        <v>0</v>
+      </c>
+      <c r="H38" s="6" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="7" t="s">
+        <v>307</v>
+      </c>
+      <c r="B39" s="6">
+        <v>1</v>
+      </c>
+      <c r="C39" s="6">
+        <v>0</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="G39" s="6">
+        <v>0</v>
+      </c>
+      <c r="H39" s="6" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="B40" s="6">
+        <v>0</v>
+      </c>
+      <c r="C40" s="6">
+        <v>0</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="G40" s="6">
+        <v>0</v>
+      </c>
+      <c r="H40" s="6" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="7" t="s">
+        <v>309</v>
+      </c>
+      <c r="B41" s="6">
+        <v>1</v>
+      </c>
+      <c r="C41" s="6">
+        <v>0</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F41" s="6">
+        <v>4</v>
+      </c>
+      <c r="G41" s="6">
+        <v>1</v>
+      </c>
+      <c r="H41" s="6" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="9" t="s">
+        <v>310</v>
+      </c>
+      <c r="B42" s="10">
+        <v>0</v>
+      </c>
+      <c r="C42" s="10">
+        <v>0</v>
+      </c>
+      <c r="E42" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="G42" s="10">
+        <v>0</v>
+      </c>
+      <c r="H42" s="10" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="9" t="s">
+        <v>311</v>
+      </c>
+      <c r="B43" s="10">
+        <v>0</v>
+      </c>
+      <c r="C43" s="10">
+        <v>0</v>
+      </c>
+      <c r="E43" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="G43" s="10">
+        <v>0</v>
+      </c>
+      <c r="H43" s="10" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="9" t="s">
+        <v>312</v>
+      </c>
+      <c r="B44" s="10">
+        <v>0</v>
+      </c>
+      <c r="C44" s="10">
+        <v>0</v>
+      </c>
+      <c r="E44" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="G44" s="10">
+        <v>0</v>
+      </c>
+      <c r="H44" s="10" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="B45" s="6">
+        <v>1</v>
+      </c>
+      <c r="C45" s="6">
+        <v>0</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="F45" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="G45" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="B46" s="6">
+        <v>0</v>
+      </c>
+      <c r="C46" s="6">
+        <v>0</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="F46" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="G46" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="B47" s="6">
+        <v>1</v>
+      </c>
+      <c r="C47" s="6">
+        <v>1</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="F47" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="G47" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="7" t="s">
+        <v>297</v>
+      </c>
+      <c r="B48" s="6">
+        <v>0</v>
+      </c>
+      <c r="C48" s="6">
+        <v>0</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>298</v>
+      </c>
+      <c r="E48" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="G48" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="6"/>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="6"/>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="6"/>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="6"/>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="6"/>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="6"/>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="6"/>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="6"/>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="6"/>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Parse zoning and export
</commit_message>
<xml_diff>
--- a/references/Zoning_Parser_Codebook.xlsx
+++ b/references/Zoning_Parser_Codebook.xlsx
@@ -18,6 +18,9 @@
     <sheet name="specific_plan" sheetId="2" r:id="rId4"/>
     <sheet name="use_for_parse_fails" sheetId="7" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">use_for_parse_fails!$A$1:$H$44</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -28,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="317">
   <si>
     <t>O</t>
   </si>
@@ -1056,17 +1059,17 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2993,16 +2996,16 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H61"/>
+  <dimension ref="A1:H57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M20" sqref="M20"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.5703125" style="13" customWidth="1"/>
+    <col min="1" max="1" width="29.5703125" style="9" customWidth="1"/>
     <col min="2" max="3" width="9.140625" style="6"/>
     <col min="4" max="4" width="10.42578125" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.85546875" style="6" bestFit="1" customWidth="1"/>
@@ -3038,59 +3041,68 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>258</v>
+        <v>266</v>
       </c>
       <c r="B2" s="6">
         <v>0</v>
       </c>
       <c r="C2" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>259</v>
+        <v>126</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>259</v>
+        <v>259</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>240</v>
       </c>
       <c r="G2" s="6">
         <v>0</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>260</v>
+        <v>267</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>61</v>
+        <v>268</v>
       </c>
       <c r="B3" s="6">
         <v>0</v>
       </c>
       <c r="C3" s="6">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>126</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>61</v>
+        <v>259</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>240</v>
       </c>
       <c r="G3" s="6">
         <v>0</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>261</v>
+        <v>270</v>
       </c>
       <c r="B4" s="6">
+        <v>0</v>
+      </c>
+      <c r="C4" s="6">
         <v>1</v>
       </c>
-      <c r="C4" s="6">
-        <v>0</v>
-      </c>
       <c r="D4" s="6" t="s">
-        <v>262</v>
+        <v>126</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>259</v>
@@ -3102,12 +3114,12 @@
         <v>0</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>259</v>
+        <v>271</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>263</v>
+        <v>272</v>
       </c>
       <c r="B5" s="6">
         <v>0</v>
@@ -3116,10 +3128,7 @@
         <v>0</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>264</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>259</v>
+        <v>101</v>
       </c>
       <c r="F5" s="8" t="s">
         <v>240</v>
@@ -3128,24 +3137,21 @@
         <v>0</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>259</v>
+        <v>273</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>265</v>
+        <v>274</v>
       </c>
       <c r="B6" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>262</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>259</v>
+        <v>89</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>240</v>
@@ -3153,48 +3159,42 @@
       <c r="G6" s="6">
         <v>0</v>
       </c>
-      <c r="H6" s="6" t="s">
-        <v>259</v>
-      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>266</v>
+        <v>309</v>
       </c>
       <c r="B7" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" s="6">
+        <v>0</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" s="6">
+        <v>4</v>
+      </c>
+      <c r="G7" s="6">
         <v>1</v>
       </c>
-      <c r="D7" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>259</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>240</v>
-      </c>
-      <c r="G7" s="6">
-        <v>0</v>
-      </c>
       <c r="H7" s="6" t="s">
-        <v>267</v>
+        <v>313</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="B8" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8" s="6">
         <v>1</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>126</v>
+        <v>262</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>259</v>
@@ -3206,12 +3206,12 @@
         <v>0</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>270</v>
+        <v>289</v>
       </c>
       <c r="B9" s="6">
         <v>0</v>
@@ -3220,47 +3220,50 @@
         <v>1</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>126</v>
+        <v>259</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>259</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>240</v>
+        <v>154</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>259</v>
       </c>
       <c r="G9" s="6">
         <v>0</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>271</v>
+        <v>259</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>272</v>
+        <v>287</v>
       </c>
       <c r="B10" s="6">
         <v>0</v>
       </c>
       <c r="C10" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>240</v>
+        <v>259</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>259</v>
       </c>
       <c r="G10" s="6">
         <v>0</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>274</v>
+        <v>288</v>
       </c>
       <c r="B11" s="6">
         <v>0</v>
@@ -3269,55 +3272,76 @@
         <v>0</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>240</v>
+        <v>259</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>259</v>
       </c>
       <c r="G11" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
-        <v>275</v>
-      </c>
-      <c r="B12" s="10">
-        <v>0</v>
-      </c>
-      <c r="C12" s="10">
-        <v>0</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>302</v>
-      </c>
-      <c r="G12" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
-        <v>277</v>
-      </c>
-      <c r="B13" s="10">
-        <v>0</v>
-      </c>
-      <c r="C13" s="10">
-        <v>0</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>304</v>
-      </c>
-      <c r="G13" s="10">
-        <v>0</v>
-      </c>
-      <c r="H13" s="10" t="s">
-        <v>305</v>
+      <c r="H11" s="6" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="B12" s="6">
+        <v>0</v>
+      </c>
+      <c r="C12" s="6">
+        <v>0</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="G12" s="6">
+        <v>0</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="B13" s="6">
+        <v>0</v>
+      </c>
+      <c r="C13" s="6">
+        <v>0</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="G13" s="6">
+        <v>0</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>58</v>
+        <v>299</v>
       </c>
       <c r="B14" s="6">
         <v>0</v>
@@ -3325,36 +3349,51 @@
       <c r="C14" s="6">
         <v>0</v>
       </c>
+      <c r="D14" s="6" t="s">
+        <v>259</v>
+      </c>
       <c r="E14" s="6" t="s">
-        <v>58</v>
+        <v>159</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>259</v>
       </c>
       <c r="G14" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
-        <v>279</v>
-      </c>
-      <c r="B15" s="10">
-        <v>0</v>
-      </c>
-      <c r="C15" s="10">
-        <v>0</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>278</v>
-      </c>
-      <c r="G15" s="10">
-        <v>0</v>
-      </c>
-      <c r="H15" s="10" t="s">
-        <v>276</v>
+      <c r="H14" s="6" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="B15" s="6">
+        <v>0</v>
+      </c>
+      <c r="C15" s="6">
+        <v>0</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="G15" s="6">
+        <v>0</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>60</v>
+        <v>258</v>
       </c>
       <c r="B16" s="6">
         <v>0</v>
@@ -3362,16 +3401,25 @@
       <c r="C16" s="6">
         <v>0</v>
       </c>
+      <c r="D16" s="6" t="s">
+        <v>259</v>
+      </c>
       <c r="E16" s="6" t="s">
-        <v>60</v>
+        <v>160</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>259</v>
       </c>
       <c r="G16" s="6">
         <v>0</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>59</v>
+        <v>291</v>
       </c>
       <c r="B17" s="6">
         <v>0</v>
@@ -3379,45 +3427,60 @@
       <c r="C17" s="6">
         <v>0</v>
       </c>
+      <c r="D17" s="6" t="s">
+        <v>259</v>
+      </c>
       <c r="E17" s="6" t="s">
-        <v>59</v>
+        <v>161</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>259</v>
       </c>
       <c r="G17" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
-        <v>280</v>
-      </c>
-      <c r="B18" s="10">
-        <v>0</v>
-      </c>
-      <c r="C18" s="10">
-        <v>0</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>303</v>
-      </c>
-      <c r="G18" s="10">
-        <v>0</v>
+      <c r="H17" s="6" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>307</v>
+      </c>
+      <c r="B18" s="6">
+        <v>1</v>
+      </c>
+      <c r="C18" s="6">
+        <v>0</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="G18" s="6">
+        <v>0</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>281</v>
+        <v>261</v>
       </c>
       <c r="B19" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C19" s="6">
         <v>0</v>
       </c>
+      <c r="D19" s="6" t="s">
+        <v>262</v>
+      </c>
       <c r="E19" s="6" t="s">
-        <v>281</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>259</v>
+        <v>259</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>240</v>
       </c>
       <c r="G19" s="6">
         <v>0</v>
@@ -3428,7 +3491,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>57</v>
+        <v>263</v>
       </c>
       <c r="B20" s="6">
         <v>0</v>
@@ -3437,13 +3500,13 @@
         <v>0</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>259</v>
+        <v>264</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>259</v>
+        <v>259</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>240</v>
       </c>
       <c r="G20" s="6">
         <v>0</v>
@@ -3454,7 +3517,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>47</v>
+        <v>308</v>
       </c>
       <c r="B21" s="6">
         <v>0</v>
@@ -3463,21 +3526,18 @@
         <v>0</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>259</v>
+        <v>52</v>
       </c>
       <c r="G21" s="6">
         <v>0</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>259</v>
+        <v>273</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>282</v>
+        <v>47</v>
       </c>
       <c r="B22" s="6">
         <v>0</v>
@@ -3485,11 +3545,8 @@
       <c r="C22" s="6">
         <v>0</v>
       </c>
-      <c r="D22" s="6" t="s">
-        <v>259</v>
-      </c>
       <c r="E22" s="6" t="s">
-        <v>158</v>
+        <v>47</v>
       </c>
       <c r="F22" s="6" t="s">
         <v>259</v>
@@ -3498,12 +3555,12 @@
         <v>0</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>283</v>
+        <v>259</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>62</v>
+        <v>281</v>
       </c>
       <c r="B23" s="6">
         <v>0</v>
@@ -3511,11 +3568,8 @@
       <c r="C23" s="6">
         <v>0</v>
       </c>
-      <c r="D23" s="6" t="s">
-        <v>259</v>
-      </c>
       <c r="E23" s="6" t="s">
-        <v>62</v>
+        <v>281</v>
       </c>
       <c r="F23" s="6" t="s">
         <v>259</v>
@@ -3529,7 +3583,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>284</v>
+        <v>57</v>
       </c>
       <c r="B24" s="6">
         <v>0</v>
@@ -3538,19 +3592,19 @@
         <v>0</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>92</v>
+        <v>259</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>259</v>
+        <v>57</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>231</v>
+        <v>259</v>
       </c>
       <c r="G24" s="6">
         <v>0</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>285</v>
+        <v>259</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -3581,7 +3635,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>286</v>
+        <v>297</v>
       </c>
       <c r="B26" s="6">
         <v>0</v>
@@ -3590,10 +3644,10 @@
         <v>0</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>259</v>
+        <v>298</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>160</v>
+        <v>50</v>
       </c>
       <c r="F26" s="6" t="s">
         <v>259</v>
@@ -3602,116 +3656,104 @@
         <v>0</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>283</v>
+        <v>259</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="7" t="s">
-        <v>287</v>
-      </c>
-      <c r="B27" s="6">
-        <v>0</v>
-      </c>
-      <c r="C27" s="6">
-        <v>1</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>259</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>259</v>
-      </c>
-      <c r="G27" s="6">
-        <v>0</v>
-      </c>
-      <c r="H27" s="6" t="s">
-        <v>259</v>
+      <c r="A27" s="10" t="s">
+        <v>300</v>
+      </c>
+      <c r="B27" s="11">
+        <v>0</v>
+      </c>
+      <c r="C27" s="11">
+        <v>0</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>259</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="F27" s="11" t="s">
+        <v>259</v>
+      </c>
+      <c r="G27" s="11">
+        <v>0</v>
+      </c>
+      <c r="H27" s="11" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="B28" s="6">
-        <v>0</v>
-      </c>
-      <c r="C28" s="6">
-        <v>0</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>259</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="F28" s="6" t="s">
-        <v>259</v>
-      </c>
-      <c r="G28" s="6">
-        <v>0</v>
-      </c>
-      <c r="H28" s="6" t="s">
-        <v>283</v>
+      <c r="A28" s="10" t="s">
+        <v>310</v>
+      </c>
+      <c r="B28" s="11">
+        <v>0</v>
+      </c>
+      <c r="C28" s="11">
+        <v>0</v>
+      </c>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11">
+        <v>0</v>
+      </c>
+      <c r="H28" s="11" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="7" t="s">
-        <v>289</v>
-      </c>
-      <c r="B29" s="6">
-        <v>0</v>
-      </c>
-      <c r="C29" s="6">
-        <v>1</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>259</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="F29" s="6" t="s">
-        <v>259</v>
-      </c>
-      <c r="G29" s="6">
-        <v>0</v>
-      </c>
-      <c r="H29" s="6" t="s">
-        <v>259</v>
+      <c r="A29" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="B29" s="11">
+        <v>0</v>
+      </c>
+      <c r="C29" s="11">
+        <v>0</v>
+      </c>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11">
+        <v>0</v>
+      </c>
+      <c r="H29" s="11" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="7" t="s">
-        <v>290</v>
-      </c>
-      <c r="B30" s="6">
-        <v>0</v>
-      </c>
-      <c r="C30" s="6">
-        <v>0</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>259</v>
-      </c>
-      <c r="E30" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="F30" s="6" t="s">
-        <v>259</v>
-      </c>
-      <c r="G30" s="6">
-        <v>0</v>
-      </c>
-      <c r="H30" s="6" t="s">
-        <v>260</v>
+      <c r="A30" s="10" t="s">
+        <v>312</v>
+      </c>
+      <c r="B30" s="11">
+        <v>0</v>
+      </c>
+      <c r="C30" s="11">
+        <v>0</v>
+      </c>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11">
+        <v>0</v>
+      </c>
+      <c r="H30" s="11" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>291</v>
+        <v>153</v>
       </c>
       <c r="B31" s="6">
         <v>0</v>
@@ -3723,7 +3765,7 @@
         <v>259</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="F31" s="6" t="s">
         <v>259</v>
@@ -3732,193 +3774,195 @@
         <v>0</v>
       </c>
       <c r="H31" s="6" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
-        <v>292</v>
+        <v>62</v>
+      </c>
+      <c r="B32" s="6">
+        <v>0</v>
+      </c>
+      <c r="C32" s="6">
+        <v>0</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>259</v>
       </c>
       <c r="G32" s="6">
         <v>0</v>
+      </c>
+      <c r="H32" s="6" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="B33" s="6">
+        <v>0</v>
+      </c>
+      <c r="C33" s="6">
+        <v>0</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="G33" s="6">
+        <v>0</v>
+      </c>
+      <c r="H33" s="6" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="7" t="s">
         <v>293</v>
       </c>
-      <c r="B33" s="6">
-        <v>0</v>
-      </c>
-      <c r="C33" s="6">
-        <v>0</v>
-      </c>
-      <c r="D33" s="6" t="s">
+      <c r="B34" s="6">
+        <v>0</v>
+      </c>
+      <c r="C34" s="6">
+        <v>0</v>
+      </c>
+      <c r="D34" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="E33" s="6" t="s">
-        <v>259</v>
-      </c>
-      <c r="F33" s="8" t="s">
+      <c r="E34" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="F34" s="8" t="s">
         <v>240</v>
       </c>
-      <c r="G33" s="6">
-        <v>0</v>
-      </c>
-      <c r="H33" s="6" t="s">
+      <c r="G34" s="6">
+        <v>0</v>
+      </c>
+      <c r="H34" s="6" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="34" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="11" t="s">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="12" t="s">
         <v>295</v>
       </c>
-      <c r="B34" s="12">
-        <v>0</v>
-      </c>
-      <c r="C34" s="12">
-        <v>0</v>
-      </c>
-      <c r="D34" s="12" t="s">
+      <c r="B35" s="13">
+        <v>0</v>
+      </c>
+      <c r="C35" s="13">
+        <v>0</v>
+      </c>
+      <c r="D35" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="F34" s="12" t="s">
-        <v>259</v>
-      </c>
-      <c r="G34" s="12">
-        <v>0</v>
-      </c>
-      <c r="H34" s="12" t="s">
+      <c r="E35" s="13"/>
+      <c r="F35" s="13" t="s">
+        <v>259</v>
+      </c>
+      <c r="G35" s="13">
+        <v>0</v>
+      </c>
+      <c r="H35" s="13" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="7" t="s">
-        <v>297</v>
-      </c>
-      <c r="B35" s="6">
-        <v>0</v>
-      </c>
-      <c r="C35" s="6">
-        <v>0</v>
-      </c>
-      <c r="D35" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="E35" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="F35" s="6" t="s">
-        <v>259</v>
-      </c>
-      <c r="G35" s="6">
-        <v>0</v>
-      </c>
-      <c r="H35" s="6" t="s">
-        <v>259</v>
-      </c>
-    </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="7" t="s">
-        <v>299</v>
-      </c>
-      <c r="B36" s="6">
-        <v>0</v>
-      </c>
-      <c r="C36" s="6">
-        <v>0</v>
-      </c>
-      <c r="D36" s="6" t="s">
-        <v>259</v>
-      </c>
-      <c r="E36" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="F36" s="6" t="s">
-        <v>259</v>
-      </c>
-      <c r="G36" s="6">
-        <v>0</v>
-      </c>
-      <c r="H36" s="6" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="9" t="s">
-        <v>300</v>
-      </c>
-      <c r="B37" s="10">
-        <v>0</v>
-      </c>
-      <c r="C37" s="10">
-        <v>0</v>
-      </c>
-      <c r="D37" s="10" t="s">
-        <v>259</v>
-      </c>
-      <c r="E37" s="10" t="s">
-        <v>152</v>
-      </c>
-      <c r="F37" s="10" t="s">
-        <v>259</v>
-      </c>
-      <c r="G37" s="10">
-        <v>0</v>
-      </c>
-      <c r="H37" s="10" t="s">
-        <v>301</v>
+      <c r="A36" s="10" t="s">
+        <v>279</v>
+      </c>
+      <c r="B36" s="11">
+        <v>0</v>
+      </c>
+      <c r="C36" s="11">
+        <v>0</v>
+      </c>
+      <c r="D36" s="11"/>
+      <c r="E36" s="11" t="s">
+        <v>278</v>
+      </c>
+      <c r="F36" s="11"/>
+      <c r="G36" s="11">
+        <v>0</v>
+      </c>
+      <c r="H36" s="11" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="B37" s="11">
+        <v>0</v>
+      </c>
+      <c r="C37" s="11">
+        <v>0</v>
+      </c>
+      <c r="D37" s="11"/>
+      <c r="E37" s="11" t="s">
+        <v>304</v>
+      </c>
+      <c r="F37" s="11"/>
+      <c r="G37" s="11">
+        <v>0</v>
+      </c>
+      <c r="H37" s="11" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="B38" s="6">
-        <v>0</v>
-      </c>
-      <c r="C38" s="6">
-        <v>0</v>
-      </c>
-      <c r="D38" s="6" t="s">
-        <v>259</v>
-      </c>
-      <c r="E38" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="F38" s="6" t="s">
-        <v>259</v>
-      </c>
-      <c r="G38" s="6">
-        <v>0</v>
-      </c>
-      <c r="H38" s="6" t="s">
-        <v>259</v>
-      </c>
+      <c r="A38" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="B38" s="11">
+        <v>0</v>
+      </c>
+      <c r="C38" s="11">
+        <v>0</v>
+      </c>
+      <c r="D38" s="11"/>
+      <c r="E38" s="11" t="s">
+        <v>303</v>
+      </c>
+      <c r="F38" s="11"/>
+      <c r="G38" s="11">
+        <v>0</v>
+      </c>
+      <c r="H38" s="11"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>307</v>
+        <v>58</v>
       </c>
       <c r="B39" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C39" s="6">
         <v>0</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="G39" s="6">
         <v>0</v>
-      </c>
-      <c r="H39" s="6" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
-        <v>308</v>
+        <v>59</v>
       </c>
       <c r="B40" s="6">
         <v>0</v>
@@ -3927,177 +3971,85 @@
         <v>0</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="G40" s="6">
         <v>0</v>
-      </c>
-      <c r="H40" s="6" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
-        <v>309</v>
+        <v>60</v>
       </c>
       <c r="B41" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C41" s="6">
         <v>0</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="F41" s="6">
-        <v>4</v>
+        <v>60</v>
       </c>
       <c r="G41" s="6">
-        <v>1</v>
-      </c>
-      <c r="H41" s="6" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="9" t="s">
-        <v>310</v>
-      </c>
-      <c r="B42" s="10">
-        <v>0</v>
-      </c>
-      <c r="C42" s="10">
-        <v>0</v>
-      </c>
-      <c r="E42" s="10" t="s">
-        <v>152</v>
-      </c>
-      <c r="G42" s="10">
-        <v>0</v>
-      </c>
-      <c r="H42" s="10" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="9" t="s">
-        <v>311</v>
-      </c>
-      <c r="B43" s="10">
-        <v>0</v>
-      </c>
-      <c r="C43" s="10">
-        <v>0</v>
-      </c>
-      <c r="E43" s="10" t="s">
-        <v>152</v>
-      </c>
-      <c r="G43" s="10">
-        <v>0</v>
-      </c>
-      <c r="H43" s="10" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="9" t="s">
-        <v>312</v>
-      </c>
-      <c r="B44" s="10">
-        <v>0</v>
-      </c>
-      <c r="C44" s="10">
-        <v>0</v>
-      </c>
-      <c r="E44" s="10" t="s">
-        <v>152</v>
-      </c>
-      <c r="G44" s="10">
-        <v>0</v>
-      </c>
-      <c r="H44" s="10" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="7" t="s">
-        <v>261</v>
-      </c>
-      <c r="B45" s="6">
-        <v>1</v>
-      </c>
-      <c r="C45" s="6">
-        <v>0</v>
-      </c>
-      <c r="D45" s="6" t="s">
-        <v>262</v>
-      </c>
-      <c r="F45" s="8" t="s">
-        <v>240</v>
-      </c>
-      <c r="G45" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="7" t="s">
-        <v>263</v>
-      </c>
-      <c r="B46" s="6">
-        <v>0</v>
-      </c>
-      <c r="C46" s="6">
-        <v>0</v>
-      </c>
-      <c r="D46" s="6" t="s">
-        <v>264</v>
-      </c>
-      <c r="F46" s="8" t="s">
-        <v>240</v>
-      </c>
-      <c r="G46" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="7" t="s">
-        <v>265</v>
-      </c>
-      <c r="B47" s="6">
-        <v>1</v>
-      </c>
-      <c r="C47" s="6">
-        <v>1</v>
-      </c>
-      <c r="D47" s="6" t="s">
-        <v>262</v>
-      </c>
-      <c r="F47" s="8" t="s">
-        <v>240</v>
-      </c>
-      <c r="G47" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B42" s="6">
+        <v>0</v>
+      </c>
+      <c r="C42" s="6">
+        <v>0</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="G42" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="10" t="s">
+        <v>275</v>
+      </c>
+      <c r="B43" s="11">
+        <v>0</v>
+      </c>
+      <c r="C43" s="11">
+        <v>0</v>
+      </c>
+      <c r="D43" s="11"/>
+      <c r="E43" s="11" t="s">
+        <v>302</v>
+      </c>
+      <c r="F43" s="11"/>
+      <c r="G43" s="11">
+        <v>0</v>
+      </c>
+      <c r="H43" s="11"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="7" t="s">
+        <v>292</v>
+      </c>
+      <c r="G44" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="7" t="s">
-        <v>297</v>
-      </c>
-      <c r="B48" s="6">
-        <v>0</v>
-      </c>
-      <c r="C48" s="6">
-        <v>0</v>
-      </c>
-      <c r="D48" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="E48" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="G48" s="6">
-        <v>0</v>
-      </c>
+      <c r="A48" s="6"/>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="6"/>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="6"/>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="6"/>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="6"/>
@@ -4117,19 +4069,12 @@
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="6"/>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" s="6"/>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" s="6"/>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" s="6"/>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61" s="6"/>
-    </row>
   </sheetData>
+  <autoFilter ref="A1:H44">
+    <sortState ref="A2:H48">
+      <sortCondition ref="A2:A48"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>